<commit_message>
Fixed a formatting issue in the date column of final dataset
</commit_message>
<xml_diff>
--- a/news_articles/data/final_dataset.xlsx
+++ b/news_articles/data/final_dataset.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -893,7 +893,7 @@
   <dimension ref="A1:J194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J194"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,7 @@
         <v>1452484</v>
       </c>
       <c r="I2">
-        <f>G2-D2</f>
+        <f t="shared" ref="I2:I33" si="0">G2-D2</f>
         <v>5.9099999999999682</v>
       </c>
       <c r="J2">
@@ -995,11 +995,11 @@
         <v>1452484</v>
       </c>
       <c r="I3">
-        <f>G3-D3</f>
+        <f t="shared" si="0"/>
         <v>5.9099999999999682</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" si="0">IF(I3&lt;0, 0, 1)</f>
+        <f t="shared" ref="J3:J66" si="1">IF(I3&lt;0, 0, 1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1029,11 +1029,11 @@
         <v>1394223</v>
       </c>
       <c r="I4">
-        <f>G4-D4</f>
+        <f t="shared" si="0"/>
         <v>4.8099999999999454</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1063,11 +1063,11 @@
         <v>1394223</v>
       </c>
       <c r="I5">
-        <f>G5-D5</f>
+        <f t="shared" si="0"/>
         <v>4.8099999999999454</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1097,11 +1097,11 @@
         <v>1394223</v>
       </c>
       <c r="I6">
-        <f>G6-D6</f>
+        <f t="shared" si="0"/>
         <v>4.8099999999999454</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1131,11 +1131,11 @@
         <v>1394223</v>
       </c>
       <c r="I7">
-        <f>G7-D7</f>
+        <f t="shared" si="0"/>
         <v>4.8099999999999454</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1165,11 +1165,11 @@
         <v>1690689</v>
       </c>
       <c r="I8">
-        <f>G8-D8</f>
+        <f t="shared" si="0"/>
         <v>-5.6200000000000045</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1199,11 +1199,11 @@
         <v>1690689</v>
       </c>
       <c r="I9">
-        <f>G9-D9</f>
+        <f t="shared" si="0"/>
         <v>-5.6200000000000045</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1233,11 +1233,11 @@
         <v>1690689</v>
       </c>
       <c r="I10">
-        <f>G10-D10</f>
+        <f t="shared" si="0"/>
         <v>-5.6200000000000045</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1267,11 +1267,11 @@
         <v>1760966</v>
       </c>
       <c r="I11">
-        <f>G11-D11</f>
+        <f t="shared" si="0"/>
         <v>10.190000000000055</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1301,11 +1301,11 @@
         <v>1488059</v>
       </c>
       <c r="I12">
-        <f>G12-D12</f>
+        <f t="shared" si="0"/>
         <v>3.9399999999999409</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1335,11 +1335,11 @@
         <v>1488059</v>
       </c>
       <c r="I13">
-        <f>G13-D13</f>
+        <f t="shared" si="0"/>
         <v>3.9399999999999409</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1369,11 +1369,11 @@
         <v>1488059</v>
       </c>
       <c r="I14">
-        <f>G14-D14</f>
+        <f t="shared" si="0"/>
         <v>3.9399999999999409</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1403,11 +1403,11 @@
         <v>1821914</v>
       </c>
       <c r="I15">
-        <f>G15-D15</f>
+        <f t="shared" si="0"/>
         <v>9.2899999999999636</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1437,11 +1437,11 @@
         <v>1821914</v>
       </c>
       <c r="I16">
-        <f>G16-D16</f>
+        <f t="shared" si="0"/>
         <v>9.2899999999999636</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1471,11 +1471,11 @@
         <v>1821914</v>
       </c>
       <c r="I17">
-        <f>G17-D17</f>
+        <f t="shared" si="0"/>
         <v>9.2899999999999636</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1505,11 +1505,11 @@
         <v>1821914</v>
       </c>
       <c r="I18">
-        <f>G18-D18</f>
+        <f t="shared" si="0"/>
         <v>9.2899999999999636</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1539,11 +1539,11 @@
         <v>1821914</v>
       </c>
       <c r="I19">
-        <f>G19-D19</f>
+        <f t="shared" si="0"/>
         <v>9.2899999999999636</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1573,11 +1573,11 @@
         <v>2104117</v>
       </c>
       <c r="I20">
-        <f>G20-D20</f>
+        <f t="shared" si="0"/>
         <v>4.2300000000000182</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1607,11 +1607,11 @@
         <v>2104117</v>
       </c>
       <c r="I21">
-        <f>G21-D21</f>
+        <f t="shared" si="0"/>
         <v>4.2300000000000182</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1641,11 +1641,11 @@
         <v>2104117</v>
       </c>
       <c r="I22">
-        <f>G22-D22</f>
+        <f t="shared" si="0"/>
         <v>4.2300000000000182</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1675,11 +1675,11 @@
         <v>2104117</v>
       </c>
       <c r="I23">
-        <f>G23-D23</f>
+        <f t="shared" si="0"/>
         <v>4.2300000000000182</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1709,11 +1709,11 @@
         <v>2145209</v>
       </c>
       <c r="I24">
-        <f>G24-D24</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1743,11 +1743,11 @@
         <v>2145209</v>
       </c>
       <c r="I25">
-        <f>G25-D25</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1777,11 +1777,11 @@
         <v>2145209</v>
       </c>
       <c r="I26">
-        <f>G26-D26</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1811,11 +1811,11 @@
         <v>2145209</v>
       </c>
       <c r="I27">
-        <f>G27-D27</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1845,11 +1845,11 @@
         <v>2145209</v>
       </c>
       <c r="I28">
-        <f>G28-D28</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1879,11 +1879,11 @@
         <v>2145209</v>
       </c>
       <c r="I29">
-        <f>G29-D29</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1913,11 +1913,11 @@
         <v>2145209</v>
       </c>
       <c r="I30">
-        <f>G30-D30</f>
+        <f t="shared" si="0"/>
         <v>2.2000000000000455</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1947,11 +1947,11 @@
         <v>1704150</v>
       </c>
       <c r="I31">
-        <f>G31-D31</f>
+        <f t="shared" si="0"/>
         <v>-0.32999999999992724</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1981,11 +1981,11 @@
         <v>1704150</v>
       </c>
       <c r="I32">
-        <f>G32-D32</f>
+        <f t="shared" si="0"/>
         <v>-0.32999999999992724</v>
       </c>
       <c r="J32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2015,11 +2015,11 @@
         <v>1704150</v>
       </c>
       <c r="I33">
-        <f>G33-D33</f>
+        <f t="shared" si="0"/>
         <v>-0.32999999999992724</v>
       </c>
       <c r="J33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2049,11 +2049,11 @@
         <v>1626499</v>
       </c>
       <c r="I34">
-        <f>G34-D34</f>
+        <f t="shared" ref="I34:I65" si="2">G34-D34</f>
         <v>0.50999999999999091</v>
       </c>
       <c r="J34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2083,11 +2083,11 @@
         <v>1626499</v>
       </c>
       <c r="I35">
-        <f>G35-D35</f>
+        <f t="shared" si="2"/>
         <v>0.50999999999999091</v>
       </c>
       <c r="J35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2117,11 +2117,11 @@
         <v>1626499</v>
       </c>
       <c r="I36">
-        <f>G36-D36</f>
+        <f t="shared" si="2"/>
         <v>0.50999999999999091</v>
       </c>
       <c r="J36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2151,11 +2151,11 @@
         <v>2443796</v>
       </c>
       <c r="I37">
-        <f>G37-D37</f>
+        <f t="shared" si="2"/>
         <v>-9.6000000000000227</v>
       </c>
       <c r="J37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2185,11 +2185,11 @@
         <v>1232087</v>
       </c>
       <c r="I38">
-        <f>G38-D38</f>
+        <f t="shared" si="2"/>
         <v>3.9800000000000182</v>
       </c>
       <c r="J38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2219,11 +2219,11 @@
         <v>1232087</v>
       </c>
       <c r="I39">
-        <f>G39-D39</f>
+        <f t="shared" si="2"/>
         <v>3.9800000000000182</v>
       </c>
       <c r="J39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2253,11 +2253,11 @@
         <v>1232087</v>
       </c>
       <c r="I40">
-        <f>G40-D40</f>
+        <f t="shared" si="2"/>
         <v>3.9800000000000182</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2287,11 +2287,11 @@
         <v>951014</v>
       </c>
       <c r="I41">
-        <f>G41-D41</f>
+        <f t="shared" si="2"/>
         <v>-0.34000000000003183</v>
       </c>
       <c r="J41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2321,11 +2321,11 @@
         <v>951014</v>
       </c>
       <c r="I42">
-        <f>G42-D42</f>
+        <f t="shared" si="2"/>
         <v>-0.34000000000003183</v>
       </c>
       <c r="J42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2355,11 +2355,11 @@
         <v>951014</v>
       </c>
       <c r="I43">
-        <f>G43-D43</f>
+        <f t="shared" si="2"/>
         <v>-0.34000000000003183</v>
       </c>
       <c r="J43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2389,11 +2389,11 @@
         <v>1211346</v>
       </c>
       <c r="I44">
-        <f>G44-D44</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2423,11 +2423,11 @@
         <v>1211346</v>
       </c>
       <c r="I45">
-        <f>G45-D45</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2457,11 +2457,11 @@
         <v>1211346</v>
       </c>
       <c r="I46">
-        <f>G46-D46</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2491,11 +2491,11 @@
         <v>1211346</v>
       </c>
       <c r="I47">
-        <f>G47-D47</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2525,11 +2525,11 @@
         <v>1211346</v>
       </c>
       <c r="I48">
-        <f>G48-D48</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2559,11 +2559,11 @@
         <v>1211346</v>
       </c>
       <c r="I49">
-        <f>G49-D49</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2593,11 +2593,11 @@
         <v>1211346</v>
       </c>
       <c r="I50">
-        <f>G50-D50</f>
+        <f t="shared" si="2"/>
         <v>-1.2800000000000864</v>
       </c>
       <c r="J50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2627,11 +2627,11 @@
         <v>972169</v>
       </c>
       <c r="I51">
-        <f>G51-D51</f>
+        <f t="shared" si="2"/>
         <v>-1.1000000000000227</v>
       </c>
       <c r="J51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2661,11 +2661,11 @@
         <v>972169</v>
       </c>
       <c r="I52">
-        <f>G52-D52</f>
+        <f t="shared" si="2"/>
         <v>-1.1000000000000227</v>
       </c>
       <c r="J52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2695,11 +2695,11 @@
         <v>623944</v>
       </c>
       <c r="I53">
-        <f>G53-D53</f>
+        <f t="shared" si="2"/>
         <v>-0.99000000000000909</v>
       </c>
       <c r="J53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2729,11 +2729,11 @@
         <v>623944</v>
       </c>
       <c r="I54">
-        <f>G54-D54</f>
+        <f t="shared" si="2"/>
         <v>-0.99000000000000909</v>
       </c>
       <c r="J54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2763,11 +2763,11 @@
         <v>789321</v>
       </c>
       <c r="I55">
-        <f>G55-D55</f>
+        <f t="shared" si="2"/>
         <v>0.87000000000000455</v>
       </c>
       <c r="J55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2797,11 +2797,11 @@
         <v>789321</v>
       </c>
       <c r="I56">
-        <f>G56-D56</f>
+        <f t="shared" si="2"/>
         <v>0.87000000000000455</v>
       </c>
       <c r="J56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2831,11 +2831,11 @@
         <v>789321</v>
       </c>
       <c r="I57">
-        <f>G57-D57</f>
+        <f t="shared" si="2"/>
         <v>0.87000000000000455</v>
       </c>
       <c r="J57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2865,11 +2865,11 @@
         <v>1153824</v>
       </c>
       <c r="I58">
-        <f>G58-D58</f>
+        <f t="shared" si="2"/>
         <v>-8.6500000000000909</v>
       </c>
       <c r="J58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2899,11 +2899,11 @@
         <v>1153824</v>
       </c>
       <c r="I59">
-        <f>G59-D59</f>
+        <f t="shared" si="2"/>
         <v>-8.6500000000000909</v>
       </c>
       <c r="J59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2933,11 +2933,11 @@
         <v>744272</v>
       </c>
       <c r="I60">
-        <f>G60-D60</f>
+        <f t="shared" si="2"/>
         <v>-0.54000000000007731</v>
       </c>
       <c r="J60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2967,11 +2967,11 @@
         <v>744272</v>
       </c>
       <c r="I61">
-        <f>G61-D61</f>
+        <f t="shared" si="2"/>
         <v>-0.54000000000007731</v>
       </c>
       <c r="J61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3001,11 +3001,11 @@
         <v>744272</v>
       </c>
       <c r="I62">
-        <f>G62-D62</f>
+        <f t="shared" si="2"/>
         <v>-0.54000000000007731</v>
       </c>
       <c r="J62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3035,11 +3035,11 @@
         <v>1769950</v>
       </c>
       <c r="I63">
-        <f>G63-D63</f>
+        <f t="shared" si="2"/>
         <v>-10.92999999999995</v>
       </c>
       <c r="J63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3069,11 +3069,11 @@
         <v>1769950</v>
       </c>
       <c r="I64">
-        <f>G64-D64</f>
+        <f t="shared" si="2"/>
         <v>-10.92999999999995</v>
       </c>
       <c r="J64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3103,11 +3103,11 @@
         <v>1769950</v>
       </c>
       <c r="I65">
-        <f>G65-D65</f>
+        <f t="shared" si="2"/>
         <v>-10.92999999999995</v>
       </c>
       <c r="J65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3137,11 +3137,11 @@
         <v>1657268</v>
       </c>
       <c r="I66">
-        <f>G66-D66</f>
+        <f t="shared" ref="I66:I97" si="3">G66-D66</f>
         <v>7.3300000000000409</v>
       </c>
       <c r="J66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3171,11 +3171,11 @@
         <v>1657268</v>
       </c>
       <c r="I67">
-        <f>G67-D67</f>
+        <f t="shared" si="3"/>
         <v>7.3300000000000409</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J130" si="1">IF(I67&lt;0, 0, 1)</f>
+        <f t="shared" ref="J67:J130" si="4">IF(I67&lt;0, 0, 1)</f>
         <v>1</v>
       </c>
     </row>
@@ -3205,11 +3205,11 @@
         <v>1072958</v>
       </c>
       <c r="I68">
-        <f>G68-D68</f>
+        <f t="shared" si="3"/>
         <v>-1.4600000000000364</v>
       </c>
       <c r="J68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3239,11 +3239,11 @@
         <v>1072958</v>
       </c>
       <c r="I69">
-        <f>G69-D69</f>
+        <f t="shared" si="3"/>
         <v>-1.4600000000000364</v>
       </c>
       <c r="J69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3273,11 +3273,11 @@
         <v>1335167</v>
       </c>
       <c r="I70">
-        <f>G70-D70</f>
+        <f t="shared" si="3"/>
         <v>7.9399999999999409</v>
       </c>
       <c r="J70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3307,11 +3307,11 @@
         <v>1335167</v>
       </c>
       <c r="I71">
-        <f>G71-D71</f>
+        <f t="shared" si="3"/>
         <v>7.9399999999999409</v>
       </c>
       <c r="J71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3341,11 +3341,11 @@
         <v>1640170</v>
       </c>
       <c r="I72">
-        <f>G72-D72</f>
+        <f t="shared" si="3"/>
         <v>10.889999999999986</v>
       </c>
       <c r="J72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3375,11 +3375,11 @@
         <v>1640170</v>
       </c>
       <c r="I73">
-        <f>G73-D73</f>
+        <f t="shared" si="3"/>
         <v>10.889999999999986</v>
       </c>
       <c r="J73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3409,11 +3409,11 @@
         <v>1274645</v>
       </c>
       <c r="I74">
-        <f>G74-D74</f>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="J74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3443,11 +3443,11 @@
         <v>1274645</v>
       </c>
       <c r="I75">
-        <f>G75-D75</f>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="J75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3477,11 +3477,11 @@
         <v>1274645</v>
       </c>
       <c r="I76">
-        <f>G76-D76</f>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="J76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3511,11 +3511,11 @@
         <v>1176780</v>
       </c>
       <c r="I77">
-        <f>G77-D77</f>
+        <f t="shared" si="3"/>
         <v>-3.07000000000005</v>
       </c>
       <c r="J77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3545,11 +3545,11 @@
         <v>1176780</v>
       </c>
       <c r="I78">
-        <f>G78-D78</f>
+        <f t="shared" si="3"/>
         <v>-3.07000000000005</v>
       </c>
       <c r="J78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3579,11 +3579,11 @@
         <v>1176780</v>
       </c>
       <c r="I79">
-        <f>G79-D79</f>
+        <f t="shared" si="3"/>
         <v>-3.07000000000005</v>
       </c>
       <c r="J79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3613,11 +3613,11 @@
         <v>1065936</v>
       </c>
       <c r="I80">
-        <f>G80-D80</f>
+        <f t="shared" si="3"/>
         <v>2.9099999999999682</v>
       </c>
       <c r="J80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3647,11 +3647,11 @@
         <v>1065936</v>
       </c>
       <c r="I81">
-        <f>G81-D81</f>
+        <f t="shared" si="3"/>
         <v>2.9099999999999682</v>
       </c>
       <c r="J81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3681,11 +3681,11 @@
         <v>1065936</v>
       </c>
       <c r="I82">
-        <f>G82-D82</f>
+        <f t="shared" si="3"/>
         <v>2.9099999999999682</v>
       </c>
       <c r="J82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3715,11 +3715,11 @@
         <v>1065936</v>
       </c>
       <c r="I83">
-        <f>G83-D83</f>
+        <f t="shared" si="3"/>
         <v>2.9099999999999682</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3749,11 +3749,11 @@
         <v>1065936</v>
       </c>
       <c r="I84">
-        <f>G84-D84</f>
+        <f t="shared" si="3"/>
         <v>2.9099999999999682</v>
       </c>
       <c r="J84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -3783,11 +3783,11 @@
         <v>1353057</v>
       </c>
       <c r="I85">
-        <f>G85-D85</f>
+        <f t="shared" si="3"/>
         <v>-0.77999999999997272</v>
       </c>
       <c r="J85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3817,11 +3817,11 @@
         <v>1353057</v>
       </c>
       <c r="I86">
-        <f>G86-D86</f>
+        <f t="shared" si="3"/>
         <v>-0.77999999999997272</v>
       </c>
       <c r="J86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3851,11 +3851,11 @@
         <v>1353057</v>
       </c>
       <c r="I87">
-        <f>G87-D87</f>
+        <f t="shared" si="3"/>
         <v>-0.77999999999997272</v>
       </c>
       <c r="J87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3885,11 +3885,11 @@
         <v>1353057</v>
       </c>
       <c r="I88">
-        <f>G88-D88</f>
+        <f t="shared" si="3"/>
         <v>-0.77999999999997272</v>
       </c>
       <c r="J88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3919,11 +3919,11 @@
         <v>1353057</v>
       </c>
       <c r="I89">
-        <f>G89-D89</f>
+        <f t="shared" si="3"/>
         <v>-0.77999999999997272</v>
       </c>
       <c r="J89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3953,11 +3953,11 @@
         <v>1353057</v>
       </c>
       <c r="I90">
-        <f>G90-D90</f>
+        <f t="shared" si="3"/>
         <v>-0.77999999999997272</v>
       </c>
       <c r="J90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3987,11 +3987,11 @@
         <v>1362115</v>
       </c>
       <c r="I91">
-        <f>G91-D91</f>
+        <f t="shared" si="3"/>
         <v>-2.4700000000000273</v>
       </c>
       <c r="J91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4021,11 +4021,11 @@
         <v>919325</v>
       </c>
       <c r="I92">
-        <f>G92-D92</f>
+        <f t="shared" si="3"/>
         <v>-2.9400000000000546</v>
       </c>
       <c r="J92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4055,11 +4055,11 @@
         <v>919325</v>
       </c>
       <c r="I93">
-        <f>G93-D93</f>
+        <f t="shared" si="3"/>
         <v>-2.9400000000000546</v>
       </c>
       <c r="J93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4089,11 +4089,11 @@
         <v>919325</v>
       </c>
       <c r="I94">
-        <f>G94-D94</f>
+        <f t="shared" si="3"/>
         <v>-2.9400000000000546</v>
       </c>
       <c r="J94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4123,11 +4123,11 @@
         <v>1963628</v>
       </c>
       <c r="I95">
-        <f>G95-D95</f>
+        <f t="shared" si="3"/>
         <v>12.059999999999945</v>
       </c>
       <c r="J95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4157,11 +4157,11 @@
         <v>1963628</v>
       </c>
       <c r="I96">
-        <f>G96-D96</f>
+        <f t="shared" si="3"/>
         <v>12.059999999999945</v>
       </c>
       <c r="J96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4191,11 +4191,11 @@
         <v>1963628</v>
       </c>
       <c r="I97">
-        <f>G97-D97</f>
+        <f t="shared" si="3"/>
         <v>12.059999999999945</v>
       </c>
       <c r="J97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4225,11 +4225,11 @@
         <v>1963628</v>
       </c>
       <c r="I98">
-        <f>G98-D98</f>
+        <f t="shared" ref="I98:I129" si="5">G98-D98</f>
         <v>12.059999999999945</v>
       </c>
       <c r="J98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4259,11 +4259,11 @@
         <v>1963628</v>
       </c>
       <c r="I99">
-        <f>G99-D99</f>
+        <f t="shared" si="5"/>
         <v>12.059999999999945</v>
       </c>
       <c r="J99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4293,11 +4293,11 @@
         <v>1474010</v>
       </c>
       <c r="I100">
-        <f>G100-D100</f>
+        <f t="shared" si="5"/>
         <v>1.57000000000005</v>
       </c>
       <c r="J100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4327,11 +4327,11 @@
         <v>1474010</v>
       </c>
       <c r="I101">
-        <f>G101-D101</f>
+        <f t="shared" si="5"/>
         <v>1.57000000000005</v>
       </c>
       <c r="J101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4361,11 +4361,11 @@
         <v>1627304</v>
       </c>
       <c r="I102">
-        <f>G102-D102</f>
+        <f t="shared" si="5"/>
         <v>6.0499999999999545</v>
       </c>
       <c r="J102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4395,11 +4395,11 @@
         <v>2973891</v>
       </c>
       <c r="I103">
-        <f>G103-D103</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4429,11 +4429,11 @@
         <v>2973891</v>
       </c>
       <c r="I104">
-        <f>G104-D104</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4463,11 +4463,11 @@
         <v>2973891</v>
       </c>
       <c r="I105">
-        <f>G105-D105</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4497,11 +4497,11 @@
         <v>2973891</v>
       </c>
       <c r="I106">
-        <f>G106-D106</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4531,11 +4531,11 @@
         <v>2973891</v>
       </c>
       <c r="I107">
-        <f>G107-D107</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4565,11 +4565,11 @@
         <v>2973891</v>
       </c>
       <c r="I108">
-        <f>G108-D108</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4599,11 +4599,11 @@
         <v>2973891</v>
       </c>
       <c r="I109">
-        <f>G109-D109</f>
+        <f t="shared" si="5"/>
         <v>-5.6599999999999682</v>
       </c>
       <c r="J109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4633,11 +4633,11 @@
         <v>2965771</v>
       </c>
       <c r="I110">
-        <f>G110-D110</f>
+        <f t="shared" si="5"/>
         <v>-11.400000000000091</v>
       </c>
       <c r="J110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4667,11 +4667,11 @@
         <v>2965771</v>
       </c>
       <c r="I111">
-        <f>G111-D111</f>
+        <f t="shared" si="5"/>
         <v>-11.400000000000091</v>
       </c>
       <c r="J111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4701,11 +4701,11 @@
         <v>2965771</v>
       </c>
       <c r="I112">
-        <f>G112-D112</f>
+        <f t="shared" si="5"/>
         <v>-11.400000000000091</v>
       </c>
       <c r="J112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4735,11 +4735,11 @@
         <v>2965771</v>
       </c>
       <c r="I113">
-        <f>G113-D113</f>
+        <f t="shared" si="5"/>
         <v>-11.400000000000091</v>
       </c>
       <c r="J113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4769,11 +4769,11 @@
         <v>2965771</v>
       </c>
       <c r="I114">
-        <f>G114-D114</f>
+        <f t="shared" si="5"/>
         <v>-11.400000000000091</v>
       </c>
       <c r="J114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4803,11 +4803,11 @@
         <v>2965771</v>
       </c>
       <c r="I115">
-        <f>G115-D115</f>
+        <f t="shared" si="5"/>
         <v>-11.400000000000091</v>
       </c>
       <c r="J115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4837,11 +4837,11 @@
         <v>3246573</v>
       </c>
       <c r="I116">
-        <f>G116-D116</f>
+        <f t="shared" si="5"/>
         <v>-12.339999999999918</v>
       </c>
       <c r="J116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4871,11 +4871,11 @@
         <v>3246573</v>
       </c>
       <c r="I117">
-        <f>G117-D117</f>
+        <f t="shared" si="5"/>
         <v>-12.339999999999918</v>
       </c>
       <c r="J117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4905,11 +4905,11 @@
         <v>3246573</v>
       </c>
       <c r="I118">
-        <f>G118-D118</f>
+        <f t="shared" si="5"/>
         <v>-12.339999999999918</v>
       </c>
       <c r="J118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4939,11 +4939,11 @@
         <v>3246573</v>
       </c>
       <c r="I119">
-        <f>G119-D119</f>
+        <f t="shared" si="5"/>
         <v>-12.339999999999918</v>
       </c>
       <c r="J119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4973,11 +4973,11 @@
         <v>3246573</v>
       </c>
       <c r="I120">
-        <f>G120-D120</f>
+        <f t="shared" si="5"/>
         <v>-12.339999999999918</v>
       </c>
       <c r="J120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5007,11 +5007,11 @@
         <v>3246573</v>
       </c>
       <c r="I121">
-        <f>G121-D121</f>
+        <f t="shared" si="5"/>
         <v>-12.339999999999918</v>
       </c>
       <c r="J121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5041,11 +5041,11 @@
         <v>2160556</v>
       </c>
       <c r="I122">
-        <f>G122-D122</f>
+        <f t="shared" si="5"/>
         <v>-7.0000000000050022E-2</v>
       </c>
       <c r="J122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5075,11 +5075,11 @@
         <v>2029744</v>
       </c>
       <c r="I123">
-        <f>G123-D123</f>
+        <f t="shared" si="5"/>
         <v>-3.9799999999999045</v>
       </c>
       <c r="J123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5109,11 +5109,11 @@
         <v>2029744</v>
       </c>
       <c r="I124">
-        <f>G124-D124</f>
+        <f t="shared" si="5"/>
         <v>-3.9799999999999045</v>
       </c>
       <c r="J124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5143,11 +5143,11 @@
         <v>1463448</v>
       </c>
       <c r="I125">
-        <f>G125-D125</f>
+        <f t="shared" si="5"/>
         <v>-1.5</v>
       </c>
       <c r="J125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5177,11 +5177,11 @@
         <v>1213324</v>
       </c>
       <c r="I126">
-        <f>G126-D126</f>
+        <f t="shared" si="5"/>
         <v>3.2400000000000091</v>
       </c>
       <c r="J126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5211,11 +5211,11 @@
         <v>1213324</v>
       </c>
       <c r="I127">
-        <f>G127-D127</f>
+        <f t="shared" si="5"/>
         <v>3.2400000000000091</v>
       </c>
       <c r="J127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5245,11 +5245,11 @@
         <v>1054732</v>
       </c>
       <c r="I128">
-        <f>G128-D128</f>
+        <f t="shared" si="5"/>
         <v>1.4500000000000455</v>
       </c>
       <c r="J128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5279,11 +5279,11 @@
         <v>1054732</v>
       </c>
       <c r="I129">
-        <f>G129-D129</f>
+        <f t="shared" si="5"/>
         <v>1.4500000000000455</v>
       </c>
       <c r="J129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5313,11 +5313,11 @@
         <v>1054732</v>
       </c>
       <c r="I130">
-        <f>G130-D130</f>
+        <f t="shared" ref="I130:I161" si="6">G130-D130</f>
         <v>1.4500000000000455</v>
       </c>
       <c r="J130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -5347,11 +5347,11 @@
         <v>1054732</v>
       </c>
       <c r="I131">
-        <f>G131-D131</f>
+        <f t="shared" si="6"/>
         <v>1.4500000000000455</v>
       </c>
       <c r="J131">
-        <f t="shared" ref="J131:J194" si="2">IF(I131&lt;0, 0, 1)</f>
+        <f t="shared" ref="J131:J194" si="7">IF(I131&lt;0, 0, 1)</f>
         <v>1</v>
       </c>
     </row>
@@ -5381,11 +5381,11 @@
         <v>1313617</v>
       </c>
       <c r="I132">
-        <f>G132-D132</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5415,11 +5415,11 @@
         <v>1313617</v>
       </c>
       <c r="I133">
-        <f>G133-D133</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5449,11 +5449,11 @@
         <v>1313617</v>
       </c>
       <c r="I134">
-        <f>G134-D134</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5483,11 +5483,11 @@
         <v>1313617</v>
       </c>
       <c r="I135">
-        <f>G135-D135</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5517,11 +5517,11 @@
         <v>1313617</v>
       </c>
       <c r="I136">
-        <f>G136-D136</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5551,11 +5551,11 @@
         <v>1313617</v>
       </c>
       <c r="I137">
-        <f>G137-D137</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5585,11 +5585,11 @@
         <v>1313617</v>
       </c>
       <c r="I138">
-        <f>G138-D138</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5619,11 +5619,11 @@
         <v>1313617</v>
       </c>
       <c r="I139">
-        <f>G139-D139</f>
+        <f t="shared" si="6"/>
         <v>-0.37999999999999545</v>
       </c>
       <c r="J139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5653,11 +5653,11 @@
         <v>1611039</v>
       </c>
       <c r="I140">
-        <f>G140-D140</f>
+        <f t="shared" si="6"/>
         <v>5.0500000000000682</v>
       </c>
       <c r="J140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5687,11 +5687,11 @@
         <v>1611039</v>
       </c>
       <c r="I141">
-        <f>G141-D141</f>
+        <f t="shared" si="6"/>
         <v>5.0500000000000682</v>
       </c>
       <c r="J141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5721,11 +5721,11 @@
         <v>1611039</v>
       </c>
       <c r="I142">
-        <f>G142-D142</f>
+        <f t="shared" si="6"/>
         <v>5.0500000000000682</v>
       </c>
       <c r="J142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5755,11 +5755,11 @@
         <v>1611039</v>
       </c>
       <c r="I143">
-        <f>G143-D143</f>
+        <f t="shared" si="6"/>
         <v>5.0500000000000682</v>
       </c>
       <c r="J143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5789,11 +5789,11 @@
         <v>1611039</v>
       </c>
       <c r="I144">
-        <f>G144-D144</f>
+        <f t="shared" si="6"/>
         <v>5.0500000000000682</v>
       </c>
       <c r="J144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5823,11 +5823,11 @@
         <v>1262337</v>
       </c>
       <c r="I145">
-        <f>G145-D145</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5857,11 +5857,11 @@
         <v>1262337</v>
       </c>
       <c r="I146">
-        <f>G146-D146</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5891,11 +5891,11 @@
         <v>1262337</v>
       </c>
       <c r="I147">
-        <f>G147-D147</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5925,11 +5925,11 @@
         <v>987248</v>
       </c>
       <c r="I148">
-        <f>G148-D148</f>
+        <f t="shared" si="6"/>
         <v>2.1000000000000227</v>
       </c>
       <c r="J148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5959,11 +5959,11 @@
         <v>987248</v>
       </c>
       <c r="I149">
-        <f>G149-D149</f>
+        <f t="shared" si="6"/>
         <v>2.1000000000000227</v>
       </c>
       <c r="J149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -5993,11 +5993,11 @@
         <v>987248</v>
       </c>
       <c r="I150">
-        <f>G150-D150</f>
+        <f t="shared" si="6"/>
         <v>2.1000000000000227</v>
       </c>
       <c r="J150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6027,11 +6027,11 @@
         <v>1472771</v>
       </c>
       <c r="I151">
-        <f>G151-D151</f>
+        <f t="shared" si="6"/>
         <v>1.2100000000000364</v>
       </c>
       <c r="J151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6061,11 +6061,11 @@
         <v>1472771</v>
       </c>
       <c r="I152">
-        <f>G152-D152</f>
+        <f t="shared" si="6"/>
         <v>1.2100000000000364</v>
       </c>
       <c r="J152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6095,11 +6095,11 @@
         <v>1472771</v>
       </c>
       <c r="I153">
-        <f>G153-D153</f>
+        <f t="shared" si="6"/>
         <v>1.2100000000000364</v>
       </c>
       <c r="J153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6129,11 +6129,11 @@
         <v>1472771</v>
       </c>
       <c r="I154">
-        <f>G154-D154</f>
+        <f t="shared" si="6"/>
         <v>1.2100000000000364</v>
       </c>
       <c r="J154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6163,11 +6163,11 @@
         <v>1472771</v>
       </c>
       <c r="I155">
-        <f>G155-D155</f>
+        <f t="shared" si="6"/>
         <v>1.2100000000000364</v>
       </c>
       <c r="J155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6197,11 +6197,11 @@
         <v>1472771</v>
       </c>
       <c r="I156">
-        <f>G156-D156</f>
+        <f t="shared" si="6"/>
         <v>1.2100000000000364</v>
       </c>
       <c r="J156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6231,11 +6231,11 @@
         <v>1392202</v>
       </c>
       <c r="I157">
-        <f>G157-D157</f>
+        <f t="shared" si="6"/>
         <v>0.90999999999996817</v>
       </c>
       <c r="J157">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6265,11 +6265,11 @@
         <v>1392202</v>
       </c>
       <c r="I158">
-        <f>G158-D158</f>
+        <f t="shared" si="6"/>
         <v>0.90999999999996817</v>
       </c>
       <c r="J158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6299,11 +6299,11 @@
         <v>1392202</v>
       </c>
       <c r="I159">
-        <f>G159-D159</f>
+        <f t="shared" si="6"/>
         <v>0.90999999999996817</v>
       </c>
       <c r="J159">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6333,11 +6333,11 @@
         <v>1392202</v>
       </c>
       <c r="I160">
-        <f>G160-D160</f>
+        <f t="shared" si="6"/>
         <v>0.90999999999996817</v>
       </c>
       <c r="J160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6367,11 +6367,11 @@
         <v>1392202</v>
       </c>
       <c r="I161">
-        <f>G161-D161</f>
+        <f t="shared" si="6"/>
         <v>0.90999999999996817</v>
       </c>
       <c r="J161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6401,11 +6401,11 @@
         <v>1101466</v>
       </c>
       <c r="I162">
-        <f>G162-D162</f>
+        <f t="shared" ref="I162:I194" si="8">G162-D162</f>
         <v>4.7300000000000182</v>
       </c>
       <c r="J162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6435,11 +6435,11 @@
         <v>1101466</v>
       </c>
       <c r="I163">
-        <f>G163-D163</f>
+        <f t="shared" si="8"/>
         <v>4.7300000000000182</v>
       </c>
       <c r="J163">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6469,11 +6469,11 @@
         <v>1101466</v>
       </c>
       <c r="I164">
-        <f>G164-D164</f>
+        <f t="shared" si="8"/>
         <v>4.7300000000000182</v>
       </c>
       <c r="J164">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6503,11 +6503,11 @@
         <v>1101466</v>
       </c>
       <c r="I165">
-        <f>G165-D165</f>
+        <f t="shared" si="8"/>
         <v>4.7300000000000182</v>
       </c>
       <c r="J165">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6537,11 +6537,11 @@
         <v>1101466</v>
       </c>
       <c r="I166">
-        <f>G166-D166</f>
+        <f t="shared" si="8"/>
         <v>4.7300000000000182</v>
       </c>
       <c r="J166">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6571,11 +6571,11 @@
         <v>2260769</v>
       </c>
       <c r="I167">
-        <f>G167-D167</f>
+        <f t="shared" si="8"/>
         <v>-2.3999999999999773</v>
       </c>
       <c r="J167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6605,11 +6605,11 @@
         <v>2260769</v>
       </c>
       <c r="I168">
-        <f>G168-D168</f>
+        <f t="shared" si="8"/>
         <v>-2.3999999999999773</v>
       </c>
       <c r="J168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6639,11 +6639,11 @@
         <v>2260769</v>
       </c>
       <c r="I169">
-        <f>G169-D169</f>
+        <f t="shared" si="8"/>
         <v>-2.3999999999999773</v>
       </c>
       <c r="J169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6673,11 +6673,11 @@
         <v>2260769</v>
       </c>
       <c r="I170">
-        <f>G170-D170</f>
+        <f t="shared" si="8"/>
         <v>-2.3999999999999773</v>
       </c>
       <c r="J170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6707,11 +6707,11 @@
         <v>2260769</v>
       </c>
       <c r="I171">
-        <f>G171-D171</f>
+        <f t="shared" si="8"/>
         <v>-2.3999999999999773</v>
       </c>
       <c r="J171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6741,11 +6741,11 @@
         <v>942476</v>
       </c>
       <c r="I172">
-        <f>G172-D172</f>
+        <f t="shared" si="8"/>
         <v>-3.2200000000000273</v>
       </c>
       <c r="J172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6775,11 +6775,11 @@
         <v>942476</v>
       </c>
       <c r="I173">
-        <f>G173-D173</f>
+        <f t="shared" si="8"/>
         <v>-3.2200000000000273</v>
       </c>
       <c r="J173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6809,11 +6809,11 @@
         <v>942476</v>
       </c>
       <c r="I174">
-        <f>G174-D174</f>
+        <f t="shared" si="8"/>
         <v>-3.2200000000000273</v>
       </c>
       <c r="J174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6843,11 +6843,11 @@
         <v>942476</v>
       </c>
       <c r="I175">
-        <f>G175-D175</f>
+        <f t="shared" si="8"/>
         <v>-3.2200000000000273</v>
       </c>
       <c r="J175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6877,11 +6877,11 @@
         <v>942476</v>
       </c>
       <c r="I176">
-        <f>G176-D176</f>
+        <f t="shared" si="8"/>
         <v>-3.2200000000000273</v>
       </c>
       <c r="J176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6911,11 +6911,11 @@
         <v>1109037</v>
       </c>
       <c r="I177">
-        <f>G177-D177</f>
+        <f t="shared" si="8"/>
         <v>0.82999999999992724</v>
       </c>
       <c r="J177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6945,11 +6945,11 @@
         <v>1109037</v>
       </c>
       <c r="I178">
-        <f>G178-D178</f>
+        <f t="shared" si="8"/>
         <v>0.82999999999992724</v>
       </c>
       <c r="J178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6979,11 +6979,11 @@
         <v>1109037</v>
       </c>
       <c r="I179">
-        <f>G179-D179</f>
+        <f t="shared" si="8"/>
         <v>0.82999999999992724</v>
       </c>
       <c r="J179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7013,11 +7013,11 @@
         <v>1037630</v>
       </c>
       <c r="I180">
-        <f>G180-D180</f>
+        <f t="shared" si="8"/>
         <v>4.5099999999999909</v>
       </c>
       <c r="J180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7047,11 +7047,11 @@
         <v>1037630</v>
       </c>
       <c r="I181">
-        <f>G181-D181</f>
+        <f t="shared" si="8"/>
         <v>4.5099999999999909</v>
       </c>
       <c r="J181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7081,11 +7081,11 @@
         <v>989773</v>
       </c>
       <c r="I182">
-        <f>G182-D182</f>
+        <f t="shared" si="8"/>
         <v>1.8600000000000136</v>
       </c>
       <c r="J182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7115,11 +7115,11 @@
         <v>989773</v>
       </c>
       <c r="I183">
-        <f>G183-D183</f>
+        <f t="shared" si="8"/>
         <v>1.8600000000000136</v>
       </c>
       <c r="J183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7149,11 +7149,11 @@
         <v>989773</v>
       </c>
       <c r="I184">
-        <f>G184-D184</f>
+        <f t="shared" si="8"/>
         <v>1.8600000000000136</v>
       </c>
       <c r="J184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7183,11 +7183,11 @@
         <v>989773</v>
       </c>
       <c r="I185">
-        <f>G185-D185</f>
+        <f t="shared" si="8"/>
         <v>1.8600000000000136</v>
       </c>
       <c r="J185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7217,11 +7217,11 @@
         <v>989773</v>
       </c>
       <c r="I186">
-        <f>G186-D186</f>
+        <f t="shared" si="8"/>
         <v>1.8600000000000136</v>
       </c>
       <c r="J186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7251,11 +7251,11 @@
         <v>989773</v>
       </c>
       <c r="I187">
-        <f>G187-D187</f>
+        <f t="shared" si="8"/>
         <v>1.8600000000000136</v>
       </c>
       <c r="J187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7285,11 +7285,11 @@
         <v>1261517</v>
       </c>
       <c r="I188">
-        <f>G188-D188</f>
+        <f t="shared" si="8"/>
         <v>2.67999999999995</v>
       </c>
       <c r="J188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7319,11 +7319,11 @@
         <v>1261517</v>
       </c>
       <c r="I189">
-        <f>G189-D189</f>
+        <f t="shared" si="8"/>
         <v>2.67999999999995</v>
       </c>
       <c r="J189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7353,11 +7353,11 @@
         <v>1704024</v>
       </c>
       <c r="I190">
-        <f>G190-D190</f>
+        <f t="shared" si="8"/>
         <v>-2.9999999999972715E-2</v>
       </c>
       <c r="J190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7387,11 +7387,11 @@
         <v>1704024</v>
       </c>
       <c r="I191">
-        <f>G191-D191</f>
+        <f t="shared" si="8"/>
         <v>-2.9999999999972715E-2</v>
       </c>
       <c r="J191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7421,11 +7421,11 @@
         <v>1704024</v>
       </c>
       <c r="I192">
-        <f>G192-D192</f>
+        <f t="shared" si="8"/>
         <v>-2.9999999999972715E-2</v>
       </c>
       <c r="J192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7455,11 +7455,11 @@
         <v>1704024</v>
       </c>
       <c r="I193">
-        <f>G193-D193</f>
+        <f t="shared" si="8"/>
         <v>-2.9999999999972715E-2</v>
       </c>
       <c r="J193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7489,11 +7489,11 @@
         <v>1704024</v>
       </c>
       <c r="I194">
-        <f>G194-D194</f>
+        <f t="shared" si="8"/>
         <v>-2.9999999999972715E-2</v>
       </c>
       <c r="J194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>